<commit_message>
Added NCATS multifilter testcases 1-31
</commit_message>
<xml_diff>
--- a/InputFiles/TC21_Canine_StudyNCATSCOP01-StudyType_SampleSite_FileAsso.xlsx
+++ b/InputFiles/TC21_Canine_StudyNCATSCOP01-StudyType_SampleSite_FileAsso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0302\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335E0334-595C-4396-86BD-E4C1F85E8AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19172921-DD16-434D-BF42-9834E493DCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -60,26 +60,38 @@
     <t>StudyFilesTab</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (c)&lt;--(samp:sample)
- MATCH (cf:file)-[*]-&gt;(c)
+    <t>TC21_Canine_StudyNCATSCOP01-StudyType_SampleSite_FileAsso_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC21_Canine_StudyNCATSCOP01-StudyType_SampleSite_FileAsso_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
  MATCH (f:file)--&gt;(parent)
- MATCH (cf)--&gt;(samp:sample)
-WHERE s.clinical_study_designation in ['NCATS-COP01'] and samp.sample_site in ['Femur'] and samp.summarized_sample_type in ['Primary Malignant Tumor Tissue'] and labels(parent)[0] IN ['sample']
-OPTIONAL MATCH (sf:file)--&gt;(c)
-MATCH (cf:file)-[*]-&gt;(c:case)
-RETURN
-	count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct cf) AS `Case Files`,
-    count(distinct sf) AS `Study Files`
-    </t>
+MATCH (c)&lt;--(diag:diagnosis)
+ MATCH (samp:sample)--&gt;(c)
+ WHERE  s.clinical_study_designation in ['NCATS-COP01'] and s.clinical_study_type in ['Transcriptomics']  and samp.sample_site in ['Mandible, Mucosa'] and labels(parent)[0] IN ['study']
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+  coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+order by c.case_id asc
+limit 100</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
  MATCH (f:file)--&gt;(parent)
-WHERE s.clinical_study_designation in ['NCATS-COP01'] and samp.sample_site in ['Femur'] and samp.summarized_sample_type in ['Primary Malignant Tumor Tissue'] and labels(parent)[0] IN ['sample']
+WHERE s.clinical_study_designation in ['NCATS-COP01'] and s.clinical_study_type in ['Transcriptomics'] and samp.sample_site in ['Mandible, Mucosa'] and labels(parent)[0] IN ['study']
 WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
@@ -103,7 +115,7 @@
 MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
 MATCH (r:registration)--&gt;(c)
 MATCH (f)--&gt;(samp:sample)
-WHERE s.clinical_study_designation in ['NCATS-COP01'] and samp.sample_site in ['Femur'] and samp.summarized_sample_type in ['Primary Malignant Tumor Tissue'] and labels(parent)[0] IN ['sample'] 
+WHERE s.clinical_study_designation in ['NCATS-COP01'] and s.clinical_study_type in ['Transcriptomics'] and samp.sample_site in ['Mandible, Mucosa'] and labels(parent)[0] IN ['study'] 
  MATCH (f)-[*]-&gt;(samp:sample)
 WITH
         DISTINCT f, parent, c, demo, diag, s, samp,
@@ -138,7 +150,7 @@
 MATCH (samp:sample)--&gt;(c)
 MATCH (c)&lt;--(demo:demographic)
 MATCH (f:file)--&gt;(parent)
-WHERE s.clinical_study_designation in ['NCATS-COP01'] and samp.sample_site in ['Femur'] and samp.summarized_sample_type in ['Primary Malignant Tumor Tissue'] and labels(parent)[0] IN ['sample'] 
+WHERE s.clinical_study_designation in ['NCATS-COP01'] and s.clinical_study_type in ['Transcriptomics'] and samp.sample_site in ['Mandible, Mucosa'] and labels(parent)[0] IN ['study'] 
 WITH
         DISTINCT f, c, demo, diag, s,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -163,33 +175,25 @@
   limit 100</t>
   </si>
   <si>
-    <t>TC21_Canine_StudyNCATSCOP01-StudyType_SampleSite_FileAsso_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC21_Canine_StudyNCATSCOP01-StudyType_SampleSite_FileAsso_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+    <t>MATCH (s:study)&lt;--(c:case)
+WHERE s.clinical_study_designation IN ['NCATS-COP01']
+OPTIONAL MATCH (cf:file)--&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+ MATCH (samp:sample)--&gt;(c)
  MATCH (f:file)--&gt;(parent)
-MATCH (c)&lt;--(diag:diagnosis)
- MATCH (samp:sample)--&gt;(c)
- WHERE  s.clinical_study_designation in ['NCATS-COP01'] and s.clinical_study_type in ['Transcriptomics']  and samp.sample_site in ['Mandible, Mucosa'] and labels(parent)[0] IN ['study']
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-  coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`
-order by c.case_id asc
-limit 100</t>
+where s.clinical_study_type in ['Transcriptomics'] and samp.sample_site in ['Mandible, Mucosa'] and labels(parent)[0] IN ['study']
+OPTIONAL MATCH (s)--&gt;(p:program)
+OPTIONAL MATCH (cf:file)-[*]-&gt;(c)
+OPTIONAL MATCH (p:program)--&gt;(s)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+RETURN
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct cf) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
   </si>
 </sst>
 </file>
@@ -570,7 +574,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.35"/>
@@ -604,16 +608,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="177" customHeight="1" x14ac:dyDescent="0.35">
@@ -621,16 +625,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="164.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -638,16 +642,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="204" customHeight="1" x14ac:dyDescent="0.35">
@@ -655,16 +659,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>